<commit_message>
Operational excluding DQ mapper extraction
</commit_message>
<xml_diff>
--- a/ExcelDriveSummary/TemplateDrive.xlsx
+++ b/ExcelDriveSummary/TemplateDrive.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HobbyProjects\DriveAssistant\ExcelDriveSummary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\StefanOberholzer\GitGud\DriveAssistant\ExcelDriveSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDABC132-E513-44EF-A5DC-39221BC746C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76B0770-265D-49DC-A20C-C01C426BE1C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30105" yWindow="780" windowWidth="17220" windowHeight="8850" xr2:uid="{B12B6E18-E294-4985-A977-422328ADD677}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{B12B6E18-E294-4985-A977-422328ADD677}"/>
   </bookViews>
   <sheets>
     <sheet name="Drive" sheetId="4" r:id="rId1"/>
@@ -698,31 +698,31 @@
   <dimension ref="B2:S50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.77734375" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.6640625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="9.77734375" customWidth="1"/>
-    <col min="6" max="7" width="9.77734375" style="6" customWidth="1"/>
-    <col min="8" max="8" width="2.6640625" style="6" customWidth="1"/>
-    <col min="9" max="11" width="8.88671875" style="6" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="2.6640625" style="6" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" customWidth="1"/>
+    <col min="6" max="7" width="9.7109375" style="6" customWidth="1"/>
+    <col min="8" max="8" width="2.7109375" style="6" customWidth="1"/>
+    <col min="9" max="11" width="8.85546875" style="6" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="2.7109375" style="6" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="5" style="12" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="5" style="6" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="8.33203125" style="6" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="6.21875" style="6" hidden="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.88671875" style="6"/>
+    <col min="15" max="15" width="8.28515625" style="6" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="6.28515625" style="6" hidden="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="29" t="str">
         <f ca="1">_xlfn.CONCAT("Drive Summary ", M13, " ",TEXT(TODAY(), "mmmm yyyy"))</f>
-        <v>Drive Summary Stefan July 2024</v>
+        <v>Drive Summary Stefan August 2024</v>
       </c>
       <c r="C2" s="29"/>
       <c r="D2" s="29"/>
@@ -730,7 +730,7 @@
       <c r="F2" s="29"/>
       <c r="G2" s="29"/>
     </row>
-    <row r="3" spans="2:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="29"/>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
@@ -738,7 +738,7 @@
       <c r="F3" s="29"/>
       <c r="G3" s="29"/>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
@@ -749,7 +749,7 @@
       <c r="D5"/>
       <c r="E5" s="7" t="str">
         <f ca="1">TEXT(TODAY(), "mmmm yyyy")</f>
-        <v>July 2024</v>
+        <v>August 2024</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>20</v>
@@ -769,7 +769,7 @@
       <c r="O5" s="27"/>
       <c r="P5" s="27"/>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
@@ -779,9 +779,11 @@
       <c r="E6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="23">
+        <v>330.49700000000001</v>
+      </c>
       <c r="G6" s="16">
-        <v>1381</v>
+        <v>192</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>19</v>
@@ -805,7 +807,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
@@ -818,11 +820,11 @@
       </c>
       <c r="F7" s="18">
         <f ca="1">F6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>0</v>
+        <v>2561.3517500000003</v>
       </c>
       <c r="G7" s="18">
         <f ca="1">G6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>1528.9642857142856</v>
+        <v>1488</v>
       </c>
       <c r="I7" s="1">
         <v>0</v>
@@ -846,13 +848,13 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="1">
         <f>IF($C$16, VLOOKUP($F$7,$I$7:$K$21,3,TRUE),VLOOKUP($F$6,$I$7:$K$21,3,TRUE))</f>
-        <v>300</v>
+        <v>260</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="1"/>
@@ -878,7 +880,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -917,24 +919,24 @@
       </c>
       <c r="R9" s="9"/>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="8">
         <f ca="1">SUM(C5:C9)</f>
-        <v>2700</v>
+        <v>2660</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F10" s="17">
         <f ca="1">F6/(DAY(TODAY())-1)</f>
-        <v>0</v>
+        <v>82.624250000000004</v>
       </c>
       <c r="G10" s="17">
         <f ca="1">G6/(DAY(TODAY())-1)</f>
-        <v>49.321428571428569</v>
+        <v>48</v>
       </c>
       <c r="I10" s="1">
         <v>450</v>
@@ -958,7 +960,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
       <c r="I11" s="1">
         <v>600</v>
       </c>
@@ -981,7 +983,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>3</v>
       </c>
@@ -1008,23 +1010,23 @@
       </c>
       <c r="M12" s="6"/>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="16">
-        <v>2600.06</v>
+        <v>0</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F13" s="18">
         <f>VLOOKUP(F6,I7:K21,2,TRUE)-F6</f>
-        <v>149</v>
+        <v>118.50299999999999</v>
       </c>
       <c r="G13" s="1">
         <f ca="1">50*(DAY(EOMONTH(TODAY(), 0))-DAY(TODAY()-1))</f>
-        <v>150</v>
+        <v>1350</v>
       </c>
       <c r="I13" s="1">
         <v>900</v>
@@ -1042,13 +1044,13 @@
       <c r="O13"/>
       <c r="P13"/>
     </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="8">
         <f ca="1">C13*VLOOKUP(C12,O6:P11,2,FALSE)*10</f>
-        <v>13000.3</v>
+        <v>0</v>
       </c>
       <c r="I14" s="1">
         <v>1050</v>
@@ -1066,7 +1068,7 @@
       <c r="Q14"/>
       <c r="S14" s="2"/>
     </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
       <c r="D15" s="11"/>
       <c r="I15" s="1">
         <v>1200</v>
@@ -1083,7 +1085,7 @@
       <c r="P15"/>
       <c r="Q15"/>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>27</v>
       </c>
@@ -1105,7 +1107,7 @@
       <c r="P16"/>
       <c r="Q16"/>
     </row>
-    <row r="17" spans="2:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="30" t="s">
         <v>30</v>
       </c>
@@ -1129,7 +1131,7 @@
       <c r="P17"/>
       <c r="Q17"/>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" s="30"/>
       <c r="C18" s="30"/>
       <c r="D18" s="30"/>
@@ -1151,7 +1153,7 @@
       <c r="P18"/>
       <c r="Q18"/>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" s="30"/>
       <c r="C19" s="30"/>
       <c r="D19" s="30"/>
@@ -1173,7 +1175,7 @@
       <c r="P19"/>
       <c r="Q19"/>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="25"/>
       <c r="C20" s="25"/>
       <c r="D20" s="25"/>
@@ -1194,7 +1196,7 @@
       <c r="P20"/>
       <c r="Q20"/>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" s="25"/>
       <c r="C21" s="25"/>
       <c r="D21" s="25"/>
@@ -1213,13 +1215,13 @@
       <c r="P21"/>
       <c r="Q21"/>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22" s="25"/>
       <c r="C22" s="25"/>
       <c r="D22" s="25"/>
       <c r="Q22"/>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
       <c r="M23"/>
       <c r="N23"/>
@@ -1227,133 +1229,133 @@
       <c r="P23"/>
       <c r="Q23"/>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="M24"/>
       <c r="N24"/>
       <c r="O24" s="14"/>
       <c r="P24"/>
       <c r="Q24"/>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="M25"/>
       <c r="N25"/>
       <c r="O25" s="14"/>
       <c r="P25"/>
       <c r="Q25"/>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="O26" s="2"/>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
       <c r="M27" s="6"/>
       <c r="O27" s="2"/>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
       <c r="M28" s="6"/>
       <c r="O28" s="2"/>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="J29" s="4"/>
       <c r="M29" s="6"/>
       <c r="O29" s="2"/>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="M30" s="6"/>
       <c r="O30" s="2"/>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
       <c r="E31" s="19"/>
       <c r="F31" s="19"/>
       <c r="G31" s="20"/>
       <c r="M31" s="6"/>
       <c r="O31" s="2"/>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
       <c r="E32" s="19"/>
       <c r="F32" s="21"/>
       <c r="G32" s="20"/>
       <c r="M32" s="6"/>
       <c r="O32" s="2"/>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E33" s="19"/>
       <c r="F33" s="21"/>
       <c r="G33" s="20"/>
       <c r="M33" s="6"/>
       <c r="O33" s="2"/>
     </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E34" s="19"/>
       <c r="F34" s="21"/>
       <c r="G34" s="20"/>
       <c r="K34" s="3"/>
       <c r="M34" s="6"/>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E35" s="19"/>
       <c r="F35" s="21"/>
       <c r="G35" s="20"/>
       <c r="M35" s="6"/>
     </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E36" s="19"/>
       <c r="F36" s="21"/>
       <c r="G36" s="20"/>
       <c r="M36" s="6"/>
     </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E37" s="19"/>
       <c r="F37" s="21"/>
       <c r="G37" s="20"/>
       <c r="M37" s="6"/>
     </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E38" s="19"/>
       <c r="F38" s="21"/>
       <c r="G38" s="20"/>
       <c r="M38" s="6"/>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E39" s="19"/>
       <c r="F39" s="21"/>
       <c r="G39" s="22"/>
       <c r="M39" s="6"/>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H41" s="13"/>
       <c r="M41" s="6"/>
     </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B42" s="13"/>
       <c r="M42" s="6"/>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
       <c r="M43" s="6"/>
     </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="I44" s="3"/>
       <c r="M44" s="6"/>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="M45" s="6"/>
     </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="M46" s="6"/>
     </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="M47" s="6"/>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="M48" s="6"/>
     </row>
-    <row r="49" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M49" s="6"/>
     </row>
-    <row r="50" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M50" s="6"/>
     </row>
   </sheetData>

</xml_diff>